<commit_message>
cleaned the code, added more checkes, fixed trailing stop order and they modification
</commit_message>
<xml_diff>
--- a/db/bin/real_trade_db_2024-08-30.xlsx
+++ b/db/bin/real_trade_db_2024-08-30.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X39"/>
+  <dimension ref="A1:X75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2780,7 +2780,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B28" t="n">
         <v>372</v>
@@ -2860,7 +2860,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="B29" t="n">
         <v>374</v>
@@ -2946,7 +2946,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="B30" t="n">
         <v>405</v>
@@ -3032,7 +3032,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="B31" t="n">
         <v>410</v>
@@ -3112,7 +3112,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>119</v>
+        <v>30</v>
       </c>
       <c r="B32" t="n">
         <v>436</v>
@@ -3184,7 +3184,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>120</v>
+        <v>31</v>
       </c>
       <c r="B33" t="n">
         <v>437</v>
@@ -3256,7 +3256,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>123</v>
+        <v>32</v>
       </c>
       <c r="B34" t="n">
         <v>440</v>
@@ -3328,7 +3328,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>130</v>
+        <v>33</v>
       </c>
       <c r="B35" t="n">
         <v>447</v>
@@ -3400,7 +3400,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>134</v>
+        <v>34</v>
       </c>
       <c r="B36" t="n">
         <v>451</v>
@@ -3472,7 +3472,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>136</v>
+        <v>35</v>
       </c>
       <c r="B37" t="n">
         <v>453</v>
@@ -3544,7 +3544,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>715</v>
+        <v>36</v>
       </c>
       <c r="B38" t="n">
         <v>574</v>
@@ -3567,21 +3567,23 @@
         <v>0.04</v>
       </c>
       <c r="H38" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I38" t="inlineStr"/>
+        <v>45535.02311471065</v>
+      </c>
+      <c r="I38" t="n">
+        <v>113.0516</v>
+      </c>
       <c r="J38" t="n">
-        <v>0</v>
+        <v>1356.6192</v>
       </c>
       <c r="K38" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="L38" t="n">
         <v>12</v>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N38" t="n">
@@ -3597,7 +3599,7 @@
         <v>0.15</v>
       </c>
       <c r="R38" t="n">
-        <v>0</v>
+        <v>4.231999999999853</v>
       </c>
       <c r="S38" t="inlineStr">
         <is>
@@ -3615,7 +3617,11 @@
           <t>FA1962BC1750FB2000</t>
         </is>
       </c>
-      <c r="W38" t="inlineStr"/>
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>FA1963BC8A57BB2000</t>
+        </is>
+      </c>
       <c r="X38" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
@@ -3624,7 +3630,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>742</v>
+        <v>37</v>
       </c>
       <c r="B39" t="n">
         <v>601</v>
@@ -3647,21 +3653,23 @@
         <v>0.03</v>
       </c>
       <c r="H39" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="I39" t="inlineStr"/>
+        <v>45535.01815166666</v>
+      </c>
+      <c r="I39" t="n">
+        <v>126.05</v>
+      </c>
       <c r="J39" t="n">
-        <v>0</v>
+        <v>1386.55</v>
       </c>
       <c r="K39" t="n">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="L39" t="n">
         <v>11</v>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>bought</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="N39" t="n">
@@ -3677,7 +3685,7 @@
         <v>0.15</v>
       </c>
       <c r="R39" t="n">
-        <v>0</v>
+        <v>9.570000000000064</v>
       </c>
       <c r="S39" t="inlineStr">
         <is>
@@ -3697,6 +3705,2622 @@
       </c>
       <c r="W39" t="inlineStr"/>
       <c r="X39" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>SO</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>45534.97949696759</v>
+      </c>
+      <c r="E40" t="n">
+        <v>85.33</v>
+      </c>
+      <c r="F40" t="n">
+        <v>1365.28</v>
+      </c>
+      <c r="G40" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H40" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" t="n">
+        <v>16</v>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N40" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O40" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P40" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R40" t="n">
+        <v>0</v>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>FA1963BB7AE484A000</t>
+        </is>
+      </c>
+      <c r="T40" t="inlineStr"/>
+      <c r="U40" t="inlineStr"/>
+      <c r="V40" t="inlineStr"/>
+      <c r="W40" t="inlineStr"/>
+      <c r="X40" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>CRM</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>45534.97959670139</v>
+      </c>
+      <c r="E41" t="n">
+        <v>256.96</v>
+      </c>
+      <c r="F41" t="n">
+        <v>1284.8</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H41" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" t="n">
+        <v>5</v>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N41" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O41" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P41" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R41" t="n">
+        <v>0</v>
+      </c>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>FA1963BB835284A000</t>
+        </is>
+      </c>
+      <c r="T41" t="inlineStr"/>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>FA1963BC88F33B2000</t>
+        </is>
+      </c>
+      <c r="V41" t="inlineStr">
+        <is>
+          <t>FA1963BC8947FB2000</t>
+        </is>
+      </c>
+      <c r="W41" t="inlineStr"/>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>2</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>COST</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>45534.97972408565</v>
+      </c>
+      <c r="E42" t="n">
+        <v>883.71</v>
+      </c>
+      <c r="F42" t="n">
+        <v>883.71</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" t="n">
+        <v>1</v>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N42" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P42" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R42" t="n">
+        <v>0</v>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>FA1963BB8E0DC4A000</t>
+        </is>
+      </c>
+      <c r="T42" t="inlineStr"/>
+      <c r="U42" t="inlineStr"/>
+      <c r="V42" t="inlineStr"/>
+      <c r="W42" t="inlineStr"/>
+      <c r="X42" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>3</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>SPG</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>45534.97985813658</v>
+      </c>
+      <c r="E43" t="n">
+        <v>165.48</v>
+      </c>
+      <c r="F43" t="n">
+        <v>1323.84</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H43" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" t="n">
+        <v>8</v>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N43" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P43" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R43" t="n">
+        <v>0</v>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>FA1963BB995DBB2000</t>
+        </is>
+      </c>
+      <c r="T43" t="inlineStr"/>
+      <c r="U43" t="inlineStr"/>
+      <c r="V43" t="inlineStr"/>
+      <c r="W43" t="inlineStr"/>
+      <c r="X43" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>4</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>ZTS</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>45534.98051590277</v>
+      </c>
+      <c r="E44" t="n">
+        <v>182.32</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1276.24</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H44" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" t="n">
+        <v>7</v>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N44" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O44" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P44" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R44" t="n">
+        <v>0</v>
+      </c>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>FA1963BBD0DE3B2000</t>
+        </is>
+      </c>
+      <c r="T44" t="inlineStr"/>
+      <c r="U44" t="inlineStr"/>
+      <c r="V44" t="inlineStr"/>
+      <c r="W44" t="inlineStr"/>
+      <c r="X44" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>5</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>CMG</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="n">
+        <v>45534.98058858796</v>
+      </c>
+      <c r="E45" t="n">
+        <v>55.4</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1440.4</v>
+      </c>
+      <c r="G45" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H45" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" t="n">
+        <v>26</v>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N45" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O45" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P45" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R45" t="n">
+        <v>0</v>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>FA1963BBD704FB2000</t>
+        </is>
+      </c>
+      <c r="T45" t="inlineStr"/>
+      <c r="U45" t="inlineStr"/>
+      <c r="V45" t="inlineStr"/>
+      <c r="W45" t="inlineStr"/>
+      <c r="X45" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>6</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>DUK</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>45534.9806642824</v>
+      </c>
+      <c r="E46" t="n">
+        <v>112.22</v>
+      </c>
+      <c r="F46" t="n">
+        <v>1346.64</v>
+      </c>
+      <c r="G46" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H46" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" t="n">
+        <v>12</v>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N46" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O46" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P46" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R46" t="n">
+        <v>0</v>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>FA1963BBDD6304A000</t>
+        </is>
+      </c>
+      <c r="T46" t="inlineStr"/>
+      <c r="U46" t="inlineStr"/>
+      <c r="V46" t="inlineStr"/>
+      <c r="W46" t="inlineStr"/>
+      <c r="X46" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>7</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>INTU</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="n">
+        <v>45534.98076986111</v>
+      </c>
+      <c r="E47" t="n">
+        <v>615.85</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1231.7</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H47" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0</v>
+      </c>
+      <c r="L47" t="n">
+        <v>2</v>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N47" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O47" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P47" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R47" t="n">
+        <v>0</v>
+      </c>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>FA1963BBE64B7B2000</t>
+        </is>
+      </c>
+      <c r="T47" t="inlineStr"/>
+      <c r="U47" t="inlineStr"/>
+      <c r="V47" t="inlineStr"/>
+      <c r="W47" t="inlineStr"/>
+      <c r="X47" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>8</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>EXC</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="n">
+        <v>45534.98083173611</v>
+      </c>
+      <c r="E48" t="n">
+        <v>37.75</v>
+      </c>
+      <c r="F48" t="n">
+        <v>1434.5</v>
+      </c>
+      <c r="G48" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H48" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0</v>
+      </c>
+      <c r="L48" t="n">
+        <v>38</v>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N48" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O48" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P48" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R48" t="n">
+        <v>0</v>
+      </c>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>FA1963BBEB83BB2000</t>
+        </is>
+      </c>
+      <c r="T48" t="inlineStr"/>
+      <c r="U48" t="inlineStr"/>
+      <c r="V48" t="inlineStr"/>
+      <c r="W48" t="inlineStr"/>
+      <c r="X48" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>9</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>SBUX</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="n">
+        <v>45534.98134196759</v>
+      </c>
+      <c r="E49" t="n">
+        <v>94.62</v>
+      </c>
+      <c r="F49" t="n">
+        <v>1419.3</v>
+      </c>
+      <c r="G49" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H49" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0</v>
+      </c>
+      <c r="L49" t="n">
+        <v>15</v>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N49" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="O49" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P49" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R49" t="n">
+        <v>0</v>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>FA1963BC1692C4A000</t>
+        </is>
+      </c>
+      <c r="T49" t="inlineStr"/>
+      <c r="U49" t="inlineStr"/>
+      <c r="V49" t="inlineStr"/>
+      <c r="W49" t="inlineStr"/>
+      <c r="X49" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>10</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>MDT</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="n">
+        <v>45534.98202662037</v>
+      </c>
+      <c r="E50" t="n">
+        <v>88.03740000000001</v>
+      </c>
+      <c r="F50" t="n">
+        <v>1408.5984</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H50" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0</v>
+      </c>
+      <c r="L50" t="n">
+        <v>16</v>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N50" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O50" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P50" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R50" t="n">
+        <v>0</v>
+      </c>
+      <c r="S50" t="inlineStr">
+        <is>
+          <t>FA1963BC50597B2000</t>
+        </is>
+      </c>
+      <c r="T50" t="inlineStr"/>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>FA1963C0DA8F7B2000</t>
+        </is>
+      </c>
+      <c r="V50" t="inlineStr">
+        <is>
+          <t>FA1963C0DAE0C4A000</t>
+        </is>
+      </c>
+      <c r="W50" t="inlineStr"/>
+      <c r="X50" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>11</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>ICE</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="n">
+        <v>45534.98241041667</v>
+      </c>
+      <c r="E51" t="n">
+        <v>160.26</v>
+      </c>
+      <c r="F51" t="n">
+        <v>1442.34</v>
+      </c>
+      <c r="G51" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H51" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="n">
+        <v>0</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0</v>
+      </c>
+      <c r="L51" t="n">
+        <v>9</v>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N51" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O51" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P51" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R51" t="n">
+        <v>0</v>
+      </c>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>FA1963BC70BBFB2000</t>
+        </is>
+      </c>
+      <c r="T51" t="inlineStr"/>
+      <c r="U51" t="inlineStr"/>
+      <c r="V51" t="inlineStr"/>
+      <c r="W51" t="inlineStr"/>
+      <c r="X51" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>12</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>STZ</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="n">
+        <v>45534.9830784375</v>
+      </c>
+      <c r="E52" t="n">
+        <v>238.03</v>
+      </c>
+      <c r="F52" t="n">
+        <v>1428.18</v>
+      </c>
+      <c r="G52" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H52" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0</v>
+      </c>
+      <c r="L52" t="n">
+        <v>6</v>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N52" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O52" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P52" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R52" t="n">
+        <v>0</v>
+      </c>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>FA1963BCA91804A000</t>
+        </is>
+      </c>
+      <c r="T52" t="inlineStr"/>
+      <c r="U52" t="inlineStr"/>
+      <c r="V52" t="inlineStr"/>
+      <c r="W52" t="inlineStr"/>
+      <c r="X52" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>13</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>PLD</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="n">
+        <v>45534.98363587963</v>
+      </c>
+      <c r="E53" t="n">
+        <v>125.18</v>
+      </c>
+      <c r="F53" t="n">
+        <v>1376.98</v>
+      </c>
+      <c r="G53" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H53" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0</v>
+      </c>
+      <c r="L53" t="n">
+        <v>11</v>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N53" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O53" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P53" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q53" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R53" t="n">
+        <v>0</v>
+      </c>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>FA1963BCD8217B2000</t>
+        </is>
+      </c>
+      <c r="T53" t="inlineStr"/>
+      <c r="U53" t="inlineStr"/>
+      <c r="V53" t="inlineStr"/>
+      <c r="W53" t="inlineStr"/>
+      <c r="X53" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>14</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>SO</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="n">
+        <v>45534.98406553241</v>
+      </c>
+      <c r="E54" t="n">
+        <v>85.33</v>
+      </c>
+      <c r="F54" t="n">
+        <v>1365.28</v>
+      </c>
+      <c r="G54" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H54" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="n">
+        <v>0</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0</v>
+      </c>
+      <c r="L54" t="n">
+        <v>16</v>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N54" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O54" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P54" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R54" t="n">
+        <v>0</v>
+      </c>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>FA1963BCFC67C4A000</t>
+        </is>
+      </c>
+      <c r="T54" t="inlineStr"/>
+      <c r="U54" t="inlineStr"/>
+      <c r="V54" t="inlineStr"/>
+      <c r="W54" t="inlineStr"/>
+      <c r="X54" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>15</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>COST</t>
+        </is>
+      </c>
+      <c r="D55" s="2" t="n">
+        <v>45534.98423450231</v>
+      </c>
+      <c r="E55" t="n">
+        <v>883.71</v>
+      </c>
+      <c r="F55" t="n">
+        <v>883.71</v>
+      </c>
+      <c r="G55" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H55" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="n">
+        <v>0</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0</v>
+      </c>
+      <c r="L55" t="n">
+        <v>1</v>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N55" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O55" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P55" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q55" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R55" t="n">
+        <v>0</v>
+      </c>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>FA1963BD0AA644A000</t>
+        </is>
+      </c>
+      <c r="T55" t="inlineStr"/>
+      <c r="U55" t="inlineStr"/>
+      <c r="V55" t="inlineStr"/>
+      <c r="W55" t="inlineStr"/>
+      <c r="X55" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>16</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>SPG</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="n">
+        <v>45534.98438402778</v>
+      </c>
+      <c r="E56" t="n">
+        <v>165.48</v>
+      </c>
+      <c r="F56" t="n">
+        <v>1323.84</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H56" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="n">
+        <v>0</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0</v>
+      </c>
+      <c r="L56" t="n">
+        <v>8</v>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N56" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O56" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P56" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q56" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R56" t="n">
+        <v>0</v>
+      </c>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>FA1963BD173F84A000</t>
+        </is>
+      </c>
+      <c r="T56" t="inlineStr"/>
+      <c r="U56" t="inlineStr"/>
+      <c r="V56" t="inlineStr"/>
+      <c r="W56" t="inlineStr"/>
+      <c r="X56" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>17</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>ZTS</t>
+        </is>
+      </c>
+      <c r="D57" s="2" t="n">
+        <v>45534.98505190972</v>
+      </c>
+      <c r="E57" t="n">
+        <v>182.32</v>
+      </c>
+      <c r="F57" t="n">
+        <v>1276.24</v>
+      </c>
+      <c r="G57" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H57" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="n">
+        <v>0</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0</v>
+      </c>
+      <c r="L57" t="n">
+        <v>7</v>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N57" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O57" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P57" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q57" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R57" t="n">
+        <v>0</v>
+      </c>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>FA1963BD4F9E44A000</t>
+        </is>
+      </c>
+      <c r="T57" t="inlineStr"/>
+      <c r="U57" t="inlineStr"/>
+      <c r="V57" t="inlineStr"/>
+      <c r="W57" t="inlineStr"/>
+      <c r="X57" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>18</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>CMG</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="n">
+        <v>45534.98513167824</v>
+      </c>
+      <c r="E58" t="n">
+        <v>55.4</v>
+      </c>
+      <c r="F58" t="n">
+        <v>1440.4</v>
+      </c>
+      <c r="G58" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H58" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0</v>
+      </c>
+      <c r="L58" t="n">
+        <v>26</v>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N58" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O58" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P58" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R58" t="n">
+        <v>0</v>
+      </c>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>FA1963BD56593B2000</t>
+        </is>
+      </c>
+      <c r="T58" t="inlineStr"/>
+      <c r="U58" t="inlineStr"/>
+      <c r="V58" t="inlineStr"/>
+      <c r="W58" t="inlineStr"/>
+      <c r="X58" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>19</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>DUK</t>
+        </is>
+      </c>
+      <c r="D59" s="2" t="n">
+        <v>45534.98520525463</v>
+      </c>
+      <c r="E59" t="n">
+        <v>112.22</v>
+      </c>
+      <c r="F59" t="n">
+        <v>1346.64</v>
+      </c>
+      <c r="G59" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H59" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0</v>
+      </c>
+      <c r="L59" t="n">
+        <v>12</v>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N59" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O59" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P59" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q59" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R59" t="n">
+        <v>0</v>
+      </c>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>FA1963BD5C8CFB2000</t>
+        </is>
+      </c>
+      <c r="T59" t="inlineStr"/>
+      <c r="U59" t="inlineStr"/>
+      <c r="V59" t="inlineStr"/>
+      <c r="W59" t="inlineStr"/>
+      <c r="X59" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>20</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>INTU</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="n">
+        <v>45534.98530614583</v>
+      </c>
+      <c r="E60" t="n">
+        <v>615.85</v>
+      </c>
+      <c r="F60" t="n">
+        <v>1231.7</v>
+      </c>
+      <c r="G60" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H60" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0</v>
+      </c>
+      <c r="L60" t="n">
+        <v>2</v>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N60" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O60" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P60" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q60" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R60" t="n">
+        <v>0</v>
+      </c>
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>FA1963BD651084A000</t>
+        </is>
+      </c>
+      <c r="T60" t="inlineStr"/>
+      <c r="U60" t="inlineStr"/>
+      <c r="V60" t="inlineStr"/>
+      <c r="W60" t="inlineStr"/>
+      <c r="X60" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>21</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>EXC</t>
+        </is>
+      </c>
+      <c r="D61" s="2" t="n">
+        <v>45534.98536799769</v>
+      </c>
+      <c r="E61" t="n">
+        <v>37.75</v>
+      </c>
+      <c r="F61" t="n">
+        <v>1434.5</v>
+      </c>
+      <c r="G61" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H61" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0</v>
+      </c>
+      <c r="L61" t="n">
+        <v>38</v>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N61" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O61" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P61" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q61" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R61" t="n">
+        <v>0</v>
+      </c>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>FA1963BD6A47FB2000</t>
+        </is>
+      </c>
+      <c r="T61" t="inlineStr"/>
+      <c r="U61" t="inlineStr"/>
+      <c r="V61" t="inlineStr"/>
+      <c r="W61" t="inlineStr"/>
+      <c r="X61" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>22</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>PLD</t>
+        </is>
+      </c>
+      <c r="D62" s="2" t="n">
+        <v>45534.9881030787</v>
+      </c>
+      <c r="E62" t="n">
+        <v>125.18</v>
+      </c>
+      <c r="F62" t="n">
+        <v>1376.98</v>
+      </c>
+      <c r="G62" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H62" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="n">
+        <v>0</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L62" t="n">
+        <v>11</v>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N62" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O62" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P62" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q62" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R62" t="n">
+        <v>0</v>
+      </c>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>FA1963BE51117B2000</t>
+        </is>
+      </c>
+      <c r="T62" t="inlineStr"/>
+      <c r="U62" t="inlineStr"/>
+      <c r="V62" t="inlineStr"/>
+      <c r="W62" t="inlineStr"/>
+      <c r="X62" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>23</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>ABT</t>
+        </is>
+      </c>
+      <c r="D63" s="2" t="n">
+        <v>45534.98836896991</v>
+      </c>
+      <c r="E63" t="n">
+        <v>112.71</v>
+      </c>
+      <c r="F63" t="n">
+        <v>1352.52</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="H63" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="n">
+        <v>0</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0</v>
+      </c>
+      <c r="L63" t="n">
+        <v>12</v>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>bought</t>
+        </is>
+      </c>
+      <c r="N63" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O63" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P63" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q63" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R63" t="n">
+        <v>0</v>
+      </c>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>FA1963BE6784BB2000</t>
+        </is>
+      </c>
+      <c r="T63" t="inlineStr"/>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>FA1963C0DBF43B2000</t>
+        </is>
+      </c>
+      <c r="V63" t="inlineStr">
+        <is>
+          <t>FA1963C0DC46BB2000</t>
+        </is>
+      </c>
+      <c r="W63" t="inlineStr"/>
+      <c r="X63" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>24</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>SO</t>
+        </is>
+      </c>
+      <c r="D64" s="2" t="n">
+        <v>45534.98856988426</v>
+      </c>
+      <c r="E64" t="n">
+        <v>85.33</v>
+      </c>
+      <c r="F64" t="n">
+        <v>1365.28</v>
+      </c>
+      <c r="G64" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H64" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="n">
+        <v>0</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0</v>
+      </c>
+      <c r="L64" t="n">
+        <v>16</v>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N64" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O64" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P64" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q64" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R64" t="n">
+        <v>0</v>
+      </c>
+      <c r="S64" t="inlineStr">
+        <is>
+          <t>FA1963BE787444A000</t>
+        </is>
+      </c>
+      <c r="T64" t="inlineStr"/>
+      <c r="U64" t="inlineStr"/>
+      <c r="V64" t="inlineStr"/>
+      <c r="W64" t="inlineStr"/>
+      <c r="X64" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>25</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>COST</t>
+        </is>
+      </c>
+      <c r="D65" s="2" t="n">
+        <v>45534.98875100695</v>
+      </c>
+      <c r="E65" t="n">
+        <v>883.71</v>
+      </c>
+      <c r="F65" t="n">
+        <v>883.71</v>
+      </c>
+      <c r="G65" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H65" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="n">
+        <v>0</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0</v>
+      </c>
+      <c r="L65" t="n">
+        <v>1</v>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N65" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O65" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P65" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q65" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R65" t="n">
+        <v>0</v>
+      </c>
+      <c r="S65" t="inlineStr">
+        <is>
+          <t>FA1963BE87BC04A000</t>
+        </is>
+      </c>
+      <c r="T65" t="inlineStr"/>
+      <c r="U65" t="inlineStr"/>
+      <c r="V65" t="inlineStr"/>
+      <c r="W65" t="inlineStr"/>
+      <c r="X65" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>26</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>SPG</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="n">
+        <v>45534.98890174768</v>
+      </c>
+      <c r="E66" t="n">
+        <v>165.48</v>
+      </c>
+      <c r="F66" t="n">
+        <v>1323.84</v>
+      </c>
+      <c r="G66" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H66" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" t="n">
+        <v>0</v>
+      </c>
+      <c r="L66" t="n">
+        <v>8</v>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>placed</t>
+        </is>
+      </c>
+      <c r="N66" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O66" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P66" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q66" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R66" t="n">
+        <v>0</v>
+      </c>
+      <c r="S66" t="inlineStr">
+        <is>
+          <t>FA1963BE947B04A000</t>
+        </is>
+      </c>
+      <c r="T66" t="inlineStr"/>
+      <c r="U66" t="inlineStr"/>
+      <c r="V66" t="inlineStr"/>
+      <c r="W66" t="inlineStr"/>
+      <c r="X66" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>27</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>ZTS</t>
+        </is>
+      </c>
+      <c r="D67" s="2" t="n">
+        <v>45534.9896006713</v>
+      </c>
+      <c r="E67" t="n">
+        <v>182.32</v>
+      </c>
+      <c r="F67" t="n">
+        <v>1276.24</v>
+      </c>
+      <c r="G67" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H67" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="n">
+        <v>0</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0</v>
+      </c>
+      <c r="L67" t="n">
+        <v>7</v>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N67" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O67" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P67" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q67" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R67" t="n">
+        <v>0</v>
+      </c>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>FA1963BECF787B2000</t>
+        </is>
+      </c>
+      <c r="T67" t="inlineStr"/>
+      <c r="U67" t="inlineStr"/>
+      <c r="V67" t="inlineStr"/>
+      <c r="W67" t="inlineStr"/>
+      <c r="X67" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>28</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>CMG</t>
+        </is>
+      </c>
+      <c r="D68" s="2" t="n">
+        <v>45534.98969010416</v>
+      </c>
+      <c r="E68" t="n">
+        <v>55.4</v>
+      </c>
+      <c r="F68" t="n">
+        <v>1440.4</v>
+      </c>
+      <c r="G68" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H68" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="n">
+        <v>0</v>
+      </c>
+      <c r="K68" t="n">
+        <v>0</v>
+      </c>
+      <c r="L68" t="n">
+        <v>26</v>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N68" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O68" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P68" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q68" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R68" t="n">
+        <v>0</v>
+      </c>
+      <c r="S68" t="inlineStr">
+        <is>
+          <t>FA1963BED6FA7B2000</t>
+        </is>
+      </c>
+      <c r="T68" t="inlineStr"/>
+      <c r="U68" t="inlineStr"/>
+      <c r="V68" t="inlineStr"/>
+      <c r="W68" t="inlineStr"/>
+      <c r="X68" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>29</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>DUK</t>
+        </is>
+      </c>
+      <c r="D69" s="2" t="n">
+        <v>45534.98976527778</v>
+      </c>
+      <c r="E69" t="n">
+        <v>112.22</v>
+      </c>
+      <c r="F69" t="n">
+        <v>1346.64</v>
+      </c>
+      <c r="G69" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H69" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="n">
+        <v>0</v>
+      </c>
+      <c r="K69" t="n">
+        <v>0</v>
+      </c>
+      <c r="L69" t="n">
+        <v>12</v>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N69" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O69" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P69" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q69" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R69" t="n">
+        <v>0</v>
+      </c>
+      <c r="S69" t="inlineStr">
+        <is>
+          <t>FA1963BEDD5284A000</t>
+        </is>
+      </c>
+      <c r="T69" t="inlineStr"/>
+      <c r="U69" t="inlineStr"/>
+      <c r="V69" t="inlineStr"/>
+      <c r="W69" t="inlineStr"/>
+      <c r="X69" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>30</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>INTU</t>
+        </is>
+      </c>
+      <c r="D70" s="2" t="n">
+        <v>45534.98985866898</v>
+      </c>
+      <c r="E70" t="n">
+        <v>615.85</v>
+      </c>
+      <c r="F70" t="n">
+        <v>1231.7</v>
+      </c>
+      <c r="G70" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H70" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I70" t="inlineStr"/>
+      <c r="J70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K70" t="n">
+        <v>0</v>
+      </c>
+      <c r="L70" t="n">
+        <v>2</v>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N70" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O70" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P70" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q70" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R70" t="n">
+        <v>0</v>
+      </c>
+      <c r="S70" t="inlineStr">
+        <is>
+          <t>FA1963BEE53004A000</t>
+        </is>
+      </c>
+      <c r="T70" t="inlineStr"/>
+      <c r="U70" t="inlineStr"/>
+      <c r="V70" t="inlineStr"/>
+      <c r="W70" t="inlineStr"/>
+      <c r="X70" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>31</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>EXC</t>
+        </is>
+      </c>
+      <c r="D71" s="2" t="n">
+        <v>45534.98992576389</v>
+      </c>
+      <c r="E71" t="n">
+        <v>37.75</v>
+      </c>
+      <c r="F71" t="n">
+        <v>1434.5</v>
+      </c>
+      <c r="G71" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H71" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I71" t="inlineStr"/>
+      <c r="J71" t="n">
+        <v>0</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0</v>
+      </c>
+      <c r="L71" t="n">
+        <v>38</v>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N71" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O71" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P71" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q71" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R71" t="n">
+        <v>0</v>
+      </c>
+      <c r="S71" t="inlineStr">
+        <is>
+          <t>FA1963BEEADAFB2000</t>
+        </is>
+      </c>
+      <c r="T71" t="inlineStr"/>
+      <c r="U71" t="inlineStr"/>
+      <c r="V71" t="inlineStr"/>
+      <c r="W71" t="inlineStr"/>
+      <c r="X71" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>32</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>PLD</t>
+        </is>
+      </c>
+      <c r="D72" s="2" t="n">
+        <v>45534.99249703703</v>
+      </c>
+      <c r="E72" t="n">
+        <v>125.18</v>
+      </c>
+      <c r="F72" t="n">
+        <v>1376.98</v>
+      </c>
+      <c r="G72" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H72" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I72" t="inlineStr"/>
+      <c r="J72" t="n">
+        <v>0</v>
+      </c>
+      <c r="K72" t="n">
+        <v>0</v>
+      </c>
+      <c r="L72" t="n">
+        <v>11</v>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N72" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O72" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P72" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q72" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R72" t="n">
+        <v>0</v>
+      </c>
+      <c r="S72" t="inlineStr">
+        <is>
+          <t>FA1963BFC3CEBB2000</t>
+        </is>
+      </c>
+      <c r="T72" t="inlineStr"/>
+      <c r="U72" t="inlineStr"/>
+      <c r="V72" t="inlineStr"/>
+      <c r="W72" t="inlineStr"/>
+      <c r="X72" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="n">
+        <v>33</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>SO</t>
+        </is>
+      </c>
+      <c r="D73" s="2" t="n">
+        <v>45534.99294170139</v>
+      </c>
+      <c r="E73" t="n">
+        <v>85.33</v>
+      </c>
+      <c r="F73" t="n">
+        <v>1365.28</v>
+      </c>
+      <c r="G73" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H73" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="n">
+        <v>0</v>
+      </c>
+      <c r="K73" t="n">
+        <v>0</v>
+      </c>
+      <c r="L73" t="n">
+        <v>16</v>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N73" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O73" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P73" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q73" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R73" t="n">
+        <v>0</v>
+      </c>
+      <c r="S73" t="inlineStr">
+        <is>
+          <t>FA1963BFE9523B2000</t>
+        </is>
+      </c>
+      <c r="T73" t="inlineStr"/>
+      <c r="U73" t="inlineStr"/>
+      <c r="V73" t="inlineStr"/>
+      <c r="W73" t="inlineStr"/>
+      <c r="X73" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="n">
+        <v>34</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>COST</t>
+        </is>
+      </c>
+      <c r="D74" s="2" t="n">
+        <v>45534.99312202547</v>
+      </c>
+      <c r="E74" t="n">
+        <v>883.71</v>
+      </c>
+      <c r="F74" t="n">
+        <v>883.71</v>
+      </c>
+      <c r="G74" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H74" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="n">
+        <v>0</v>
+      </c>
+      <c r="K74" t="n">
+        <v>0</v>
+      </c>
+      <c r="L74" t="n">
+        <v>1</v>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N74" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O74" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P74" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q74" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R74" t="n">
+        <v>0</v>
+      </c>
+      <c r="S74" t="inlineStr">
+        <is>
+          <t>FA1963BFF8893B2000</t>
+        </is>
+      </c>
+      <c r="T74" t="inlineStr"/>
+      <c r="U74" t="inlineStr"/>
+      <c r="V74" t="inlineStr"/>
+      <c r="W74" t="inlineStr"/>
+      <c r="X74" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="n">
+        <v>35</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>ZTS</t>
+        </is>
+      </c>
+      <c r="D75" s="2" t="n">
+        <v>45534.99392560186</v>
+      </c>
+      <c r="E75" t="n">
+        <v>182.32</v>
+      </c>
+      <c r="F75" t="n">
+        <v>1276.24</v>
+      </c>
+      <c r="G75" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H75" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="n">
+        <v>0</v>
+      </c>
+      <c r="K75" t="n">
+        <v>0</v>
+      </c>
+      <c r="L75" t="n">
+        <v>7</v>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N75" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O75" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="P75" t="n">
+        <v>1.007</v>
+      </c>
+      <c r="Q75" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R75" t="n">
+        <v>0</v>
+      </c>
+      <c r="S75" t="inlineStr">
+        <is>
+          <t>FA1963C03C577B2000</t>
+        </is>
+      </c>
+      <c r="T75" t="inlineStr"/>
+      <c r="U75" t="inlineStr"/>
+      <c r="V75" t="inlineStr"/>
+      <c r="W75" t="inlineStr"/>
+      <c r="X75" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>

</xml_diff>